<commit_message>
Library API test and JSON to POJO utility added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/createuser.xlsx
+++ b/src/test/resources/testdata/createuser.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Framework\APIJuly23Framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7368F8CE-743A-49A7-9ACC-FC190885731C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC44B2A-DB6F-4C5E-9650-7BED5150270A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{07854A8F-CF74-4293-A36C-03AF7DF69BA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{07854A8F-CF74-4293-A36C-03AF7DF69BA5}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
+    <sheet name="Library" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>name</t>
   </si>
@@ -43,6 +44,21 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>MKR</t>
+  </si>
+  <si>
+    <t>Madhuri Kulkarni</t>
   </si>
 </sst>
 </file>
@@ -396,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F52844-546F-499D-981A-2A19FC2328B9}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,4 +443,41 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83ADBD29-9B4B-49EB-83C4-2843407A522C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Docker file and added new BookStore API
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/createuser.xlsx
+++ b/src/test/resources/testdata/createuser.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Framework\APIJuly23Framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95331625-3C67-4CE6-B6B0-D8416A66B3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2EBA68-5D8C-4134-8019-18C42C5E747D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{07854A8F-CF74-4293-A36C-03AF7DF69BA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{07854A8F-CF74-4293-A36C-03AF7DF69BA5}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
     <sheet name="Library" sheetId="2" r:id="rId2"/>
     <sheet name="PetStore" sheetId="3" r:id="rId3"/>
+    <sheet name="bookstoreUser" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -111,6 +112,18 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>ashuk</t>
+  </si>
+  <si>
+    <t>Abcd@1234</t>
   </si>
 </sst>
 </file>
@@ -155,10 +168,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -550,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBEEDCF-504C-4452-AA18-52386BE294B2}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,4 +650,38 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8133BCE8-1A58-4950-A9B6-C7A51A12B180}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{E8EC0E99-4E49-4BF5-9E26-CECB270F55A0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>